<commit_message>
Imputed Values Comparison of Algorithms
</commit_message>
<xml_diff>
--- a/data_impute_project/imputation_comparison/combination_1_ABCD/A/10/seed1_imputed_comparison.xlsx
+++ b/data_impute_project/imputation_comparison/combination_1_ABCD/A/10/seed1_imputed_comparison.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,6 +459,21 @@
           <t>RF</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>KNN_Outliers_MAD</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>SVM_Outliers_MAD</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>RF_Outliers_MAD</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -478,6 +493,15 @@
       <c r="E2" t="n">
         <v>-20.61739999999999</v>
       </c>
+      <c r="F2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -497,6 +521,15 @@
       <c r="E3" t="n">
         <v>-20.18649999999997</v>
       </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -516,6 +549,15 @@
       <c r="E4" t="n">
         <v>-22.00850000000002</v>
       </c>
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -535,6 +577,15 @@
       <c r="E5" t="n">
         <v>-21.87310000000001</v>
       </c>
+      <c r="F5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -554,6 +605,15 @@
       <c r="E6" t="n">
         <v>-20.99659999999997</v>
       </c>
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -573,6 +633,15 @@
       <c r="E7" t="n">
         <v>-21.2018</v>
       </c>
+      <c r="F7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -592,6 +661,15 @@
       <c r="E8" t="n">
         <v>-20.16279999999999</v>
       </c>
+      <c r="F8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -611,6 +689,15 @@
       <c r="E9" t="n">
         <v>-22.2744</v>
       </c>
+      <c r="F9" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -630,6 +717,15 @@
       <c r="E10" t="n">
         <v>-22.51780000000002</v>
       </c>
+      <c r="F10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -649,6 +745,15 @@
       <c r="E11" t="n">
         <v>-21.4476</v>
       </c>
+      <c r="F11" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -667,6 +772,15 @@
       </c>
       <c r="E12" t="n">
         <v>-21.99830000000002</v>
+      </c>
+      <c r="F12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>